<commit_message>
feat: completed and refined Dashboard API with accurate financial data
</commit_message>
<xml_diff>
--- a/backend/income_details.xlsx
+++ b/backend/income_details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -425,31 +425,9 @@
         <v>45817.22928240741</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Freelancing</v>
-      </c>
-      <c r="B3" t="str">
-        <v>2500</v>
-      </c>
-      <c r="C3" s="1">
-        <v>45817.22928240741</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>YouTube Earning</v>
-      </c>
-      <c r="B4" t="str">
-        <v>2000</v>
-      </c>
-      <c r="C4" s="1">
-        <v>45817.22928240741</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>